<commit_message>
Adding logic for userWindow methods.  Not yet implemented.
</commit_message>
<xml_diff>
--- a/db design.xlsx
+++ b/db design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T\source\repos\Taco Shop Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F047D597-35A4-4DB0-9D3A-918D0A3393D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF9A792-63E3-4902-AF18-465E2BFF7A86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28380" yWindow="0" windowWidth="23190" windowHeight="21150" firstSheet="1" activeTab="5" xr2:uid="{25E785AC-D4AA-45E6-9162-97BB4033E61D}"/>
+    <workbookView xWindow="28380" yWindow="0" windowWidth="23190" windowHeight="21150" activeTab="5" xr2:uid="{25E785AC-D4AA-45E6-9162-97BB4033E61D}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="55">
   <si>
     <t>username</t>
   </si>
@@ -730,7 +730,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8B234B-9FD5-4FF6-9C6C-0DE10320C619}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -956,7 +956,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C14" sqref="B2:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,6 +986,9 @@
       <c r="B2" t="s">
         <v>33</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
       <c r="D2">
         <v>1</v>
       </c>
@@ -997,6 +1000,9 @@
       <c r="B3" t="s">
         <v>34</v>
       </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
@@ -1008,6 +1014,9 @@
       <c r="B4" t="s">
         <v>35</v>
       </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
       <c r="D4">
         <v>1</v>
       </c>
@@ -1019,6 +1028,9 @@
       <c r="B5" t="s">
         <v>36</v>
       </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
       <c r="D5">
         <v>1</v>
       </c>
@@ -1029,6 +1041,9 @@
       </c>
       <c r="B6" t="s">
         <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1041,6 +1056,9 @@
       <c r="B7" t="s">
         <v>38</v>
       </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
       <c r="D7">
         <v>1</v>
       </c>
@@ -1052,6 +1070,9 @@
       <c r="B8" t="s">
         <v>39</v>
       </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
       <c r="D8">
         <v>1</v>
       </c>
@@ -1063,6 +1084,9 @@
       <c r="B9" t="s">
         <v>40</v>
       </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
       <c r="D9">
         <v>1</v>
       </c>
@@ -1073,6 +1097,9 @@
       </c>
       <c r="B10" t="s">
         <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1085,6 +1112,9 @@
       <c r="B11" t="s">
         <v>42</v>
       </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
       <c r="D11">
         <v>1</v>
       </c>
@@ -1096,6 +1126,9 @@
       <c r="B12" t="s">
         <v>43</v>
       </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -1107,6 +1140,9 @@
       <c r="B13" t="s">
         <v>44</v>
       </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
       <c r="D13">
         <v>1</v>
       </c>
@@ -1117,6 +1153,9 @@
       </c>
       <c r="B14" t="s">
         <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
       </c>
       <c r="D14">
         <v>1</v>

</xml_diff>